<commit_message>
A complete log of motor speed up to 50 RPM is produced
</commit_message>
<xml_diff>
--- a/docs/Voltage_RPM.xlsx
+++ b/docs/Voltage_RPM.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a4b0d7718c8e66bb/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\EVent-ir\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="70" documentId="8_{EBD96344-D8A9-4FDC-A5D9-117174B4A214}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{921B66F3-1228-4C77-8A71-6552A5D9C3AA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055920AA-5379-4590-8AEB-52104A64CBAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{A9626766-F829-4569-82F4-CF981F7B9FB2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{A9626766-F829-4569-82F4-CF981F7B9FB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Voltage_RPM" sheetId="1" r:id="rId1"/>
     <sheet name="PWM_Voltage" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
   <si>
     <t>Voltage</t>
   </si>
@@ -47,6 +48,9 @@
   </si>
   <si>
     <t>DriverDuty</t>
+  </si>
+  <si>
+    <t>Duty Cycle</t>
   </si>
 </sst>
 </file>
@@ -603,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA9862CD-61FF-463C-8EFC-B64C705F6E5A}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,4 +870,498 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D9FA68B-8402-41CA-A083-FB7850754862}">
+  <dimension ref="A1:D34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>4.96</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>4.74</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>4.58</v>
+      </c>
+      <c r="C5">
+        <v>4.5</v>
+      </c>
+      <c r="D5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>4.46</v>
+      </c>
+      <c r="C7">
+        <v>7.5</v>
+      </c>
+      <c r="D7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>4.41</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="C9">
+        <v>9.5</v>
+      </c>
+      <c r="D9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>4.32</v>
+      </c>
+      <c r="C10">
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="C11">
+        <v>11.5</v>
+      </c>
+      <c r="D11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="C12">
+        <v>13.5</v>
+      </c>
+      <c r="D12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>4.18</v>
+      </c>
+      <c r="C13">
+        <v>15.8</v>
+      </c>
+      <c r="D13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>4.13</v>
+      </c>
+      <c r="C14">
+        <v>16</v>
+      </c>
+      <c r="D14">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>4.09</v>
+      </c>
+      <c r="C15">
+        <v>18</v>
+      </c>
+      <c r="D15">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="C16">
+        <v>20.5</v>
+      </c>
+      <c r="D16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>3.99</v>
+      </c>
+      <c r="C17">
+        <v>20.5</v>
+      </c>
+      <c r="D17">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <v>3.92</v>
+      </c>
+      <c r="C18">
+        <v>23</v>
+      </c>
+      <c r="D18">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>28</v>
+      </c>
+      <c r="B19">
+        <v>3.86</v>
+      </c>
+      <c r="C19">
+        <v>23</v>
+      </c>
+      <c r="D19">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>29</v>
+      </c>
+      <c r="B20">
+        <v>3.82</v>
+      </c>
+      <c r="C20">
+        <v>25.5</v>
+      </c>
+      <c r="D20">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>31</v>
+      </c>
+      <c r="B21">
+        <v>3.76</v>
+      </c>
+      <c r="C21">
+        <v>27.8</v>
+      </c>
+      <c r="D21">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>33</v>
+      </c>
+      <c r="B22">
+        <v>3.7</v>
+      </c>
+      <c r="C22">
+        <v>28</v>
+      </c>
+      <c r="D22">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>34</v>
+      </c>
+      <c r="B23">
+        <v>3.67</v>
+      </c>
+      <c r="C23">
+        <v>30</v>
+      </c>
+      <c r="D23">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>35</v>
+      </c>
+      <c r="B24">
+        <v>3.64</v>
+      </c>
+      <c r="C24">
+        <v>32</v>
+      </c>
+      <c r="D24">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>38</v>
+      </c>
+      <c r="B25">
+        <v>3.56</v>
+      </c>
+      <c r="C25">
+        <v>33</v>
+      </c>
+      <c r="D25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>39</v>
+      </c>
+      <c r="B26">
+        <v>3.53</v>
+      </c>
+      <c r="C26">
+        <v>35</v>
+      </c>
+      <c r="D26">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>40</v>
+      </c>
+      <c r="B27">
+        <v>3.5</v>
+      </c>
+      <c r="C27">
+        <v>37</v>
+      </c>
+      <c r="D27">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>42</v>
+      </c>
+      <c r="B28">
+        <v>3.44</v>
+      </c>
+      <c r="C28">
+        <v>37.5</v>
+      </c>
+      <c r="D28">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>44</v>
+      </c>
+      <c r="B29">
+        <v>3.39</v>
+      </c>
+      <c r="C29">
+        <v>40</v>
+      </c>
+      <c r="D29">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>47</v>
+      </c>
+      <c r="B30">
+        <v>3.3</v>
+      </c>
+      <c r="C30">
+        <v>42</v>
+      </c>
+      <c r="D30">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>51</v>
+      </c>
+      <c r="B31">
+        <v>3.2</v>
+      </c>
+      <c r="C31">
+        <v>45</v>
+      </c>
+      <c r="D31">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>54</v>
+      </c>
+      <c r="B32">
+        <v>3.1</v>
+      </c>
+      <c r="C32">
+        <v>46.5</v>
+      </c>
+      <c r="D32">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>56</v>
+      </c>
+      <c r="B33">
+        <v>3.06</v>
+      </c>
+      <c r="C33">
+        <v>48</v>
+      </c>
+      <c r="D33">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>58</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34">
+        <v>50</v>
+      </c>
+      <c r="D34">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>